<commit_message>
update template fill kabupaten
</commit_message>
<xml_diff>
--- a/template-kabupaten-fill.xlsx
+++ b/template-kabupaten-fill.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="516">
   <si>
     <t xml:space="preserve">nama_kabupaten</t>
   </si>
@@ -1499,6 +1499,75 @@
   </si>
   <si>
     <t xml:space="preserve">Kabupaten Nduga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Selatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Tenggara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Timur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Tengah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Barat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Besar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Pidie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Utara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Simeulue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Singkil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Bireuen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Barat Daya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Gayo Lues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Jaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Nagan Raya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Aceh Tamiang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Bener Meriah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kabupaten Pidie Jaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota Banda Aceh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota Sabang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota Lhokseumawe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota Langsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota Subulussalam</t>
   </si>
 </sst>
 </file>
@@ -1615,13 +1684,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C570"/>
+  <dimension ref="A1:B570"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A453" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E472" activeCellId="0" sqref="E472"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A502" activeCellId="0" sqref="A502"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.77"/>
   </cols>
@@ -5563,473 +5632,244 @@
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C493" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A493), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A493" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B493" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A494), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A494" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="B494" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A495), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A495" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B495" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C496" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A496), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A496" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B496" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A497), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A497" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B497" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C498" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A498), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A498" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="B498" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A499), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A499" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B499" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A500), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A500" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B500" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C501" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A501), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A501" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="B501" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C502" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A502), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A502" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B502" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C503" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A503), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A503" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="B503" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C504" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A504), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A504" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B504" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C505" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A505), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A505" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B505" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C506" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A506), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A506" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B506" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C507" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A507), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A507" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B507" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A508), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A508" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="B508" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C509" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A509), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A509" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B509" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C510" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A510), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A510" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="B510" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C511" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A511), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A511" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B511" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A512), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A512" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B512" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C513" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A513), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A513" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="B513" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C514" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A514), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
+      <c r="A514" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="B514" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C515" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A515), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C516" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A516), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C517" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A517), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C518" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A518), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C519" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A519), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C520" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A520), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C521" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A521), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C522" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A522), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C523" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A523), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C524" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A524), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C525" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A525), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C526" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A526), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C527" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A527), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C528" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A528), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A529), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C530" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A530), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A531), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C532" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A532), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A533), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C534" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A534), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A535), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C536" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A536), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C537" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A537), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C538" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A538), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C539" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A539), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C540" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A540), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C541" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A541), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C542" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A542), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C543" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A543), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C544" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A544), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C545" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A545), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C546" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A546), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C547" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A547), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C548" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A548), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C549" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A549), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C550" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A550), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C551" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A551), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C552" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A552), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C553" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A553), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C554" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A554), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C555" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A555), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C556" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A556), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C557" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A557), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C558" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A558), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C559" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A559), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C560" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A560), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C561" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A561), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C562" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A562), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C563" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A563), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C564" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A564), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C565" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A565), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C566" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A566), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C567" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A567), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C568" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A568), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C569" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A569), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C570" s="0" t="str">
-        <f aca="false">=PROPER(SUBSTITUTE(SUBSTITUTE(UPPER(A570), "KAB.", "Kabupaten"), "KAB ", "Kabupaten "))</f>
-        <v/>
-      </c>
-    </row>
+      <c r="A515" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="B515" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>